<commit_message>
before 1st check by I.Yamaguchi
</commit_message>
<xml_diff>
--- a/BlockPattern.xlsx
+++ b/BlockPattern.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="31900" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="2200" yWindow="900" windowWidth="35060" windowHeight="22320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="30">
   <si>
     <t>const struct BLOCK_PATTERN Bp[] = {</t>
     <phoneticPr fontId="1"/>
@@ -41,10 +41,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>, // Duration[sec]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>{</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -100,11 +96,55 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>"FLOW",</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>"SIN",</t>
+    <t>, // Duration from[sec]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>, // to</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SHORT_PATTERN::Sp_Flash__1_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SHORT_PATTERN::Sp_Flash__2_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"SIN_6",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"FLOW_6",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"FLOW_12",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"SIN_12",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SHORT_PATTERN::Sp_On_High</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>, // Num Logical chs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"ON_HIGH",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"STROBE_1",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"STROBE_2",</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -444,19 +484,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F26"/>
+  <dimension ref="A2:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD26"/>
+      <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -470,180 +510,724 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5">
+    <row r="6" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C6">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="17" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>1.5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
+    <row r="35" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
+      <c r="F35" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>0.6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>0.25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="2" t="s">
+      <c r="F46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>0.15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>0.08</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="F57" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>0.15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>0.08</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
+    <row r="67" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15">
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D75" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C79">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="D79" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17">
-        <v>0.5</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="83" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <v>1.5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
+    <row r="84" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>2</v>
+      </c>
+      <c r="E85" t="s">
+        <v>25</v>
+      </c>
+      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F86" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>13</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
brush up:Strobe pattern:cos + phase diff
</commit_message>
<xml_diff>
--- a/BlockPattern.xlsx
+++ b/BlockPattern.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32640" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="2280" yWindow="1120" windowWidth="33940" windowHeight="22220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="39">
   <si>
     <t>const struct BLOCK_PATTERN Bp[] = {</t>
     <phoneticPr fontId="1"/>
@@ -173,6 +173,14 @@
   </si>
   <si>
     <t>, // BlankProbability</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>//</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SHORT_PATTERN::Sp_cos_forFlash</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -513,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F126"/>
+  <dimension ref="A2:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD126"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -525,7 +533,7 @@
     <col min="2" max="2" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1014,7 +1022,7 @@
     </row>
     <row r="62" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C62">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -1022,7 +1030,7 @@
     </row>
     <row r="63" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C63">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="D63" t="s">
         <v>18</v>
@@ -1085,6 +1093,9 @@
       </c>
     </row>
     <row r="71" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>37</v>
+      </c>
       <c r="D71" t="s">
         <v>2</v>
       </c>
@@ -1096,64 +1107,67 @@
       </c>
     </row>
     <row r="72" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>38</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F72" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
+      <c r="F73" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>2</v>
-      </c>
-      <c r="C75" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C76">
-        <v>0.15</v>
-      </c>
-      <c r="D76" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="77" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C77">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="D77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C78">
-        <v>2</v>
+        <v>0.08</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1161,15 +1175,15 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C81" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D81" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="82" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1177,95 +1191,95 @@
         <v>30</v>
       </c>
       <c r="D82" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D83" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C83" s="3">
-        <v>0</v>
-      </c>
-      <c r="D83" t="s">
+    <row r="84" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="3">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C84" t="s">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s">
+    <row r="85" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D85" t="s">
-        <v>2</v>
-      </c>
-      <c r="E85" t="s">
+    <row r="86" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
         <v>19</v>
       </c>
-      <c r="F85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C87" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
+      <c r="F87" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C90">
-        <v>0.15</v>
-      </c>
-      <c r="D90" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="91" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C91">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="D91" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C92">
-        <v>2</v>
+        <v>0.08</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C93">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1273,15 +1287,15 @@
         <v>0</v>
       </c>
       <c r="D94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C95" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D95" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="96" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1289,34 +1303,31 @@
         <v>30</v>
       </c>
       <c r="D96" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C97" s="3">
-        <v>0</v>
-      </c>
-      <c r="D97" t="s">
+    <row r="98" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="3">
+        <v>0</v>
+      </c>
+      <c r="D98" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C98" t="s">
-        <v>2</v>
-      </c>
-      <c r="D98" t="s">
+    <row r="99" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D99" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="100" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1357,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F103" t="s">
         <v>5</v>
@@ -1397,40 +1408,43 @@
       </c>
     </row>
     <row r="107" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D107" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E107" s="2" t="s">
+      <c r="D107" t="s">
+        <v>2</v>
+      </c>
+      <c r="E107" t="s">
+        <v>20</v>
+      </c>
+      <c r="F107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C108" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B109" t="s">
+      <c r="F108" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C109" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>2</v>
-      </c>
-      <c r="C110" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C111">
-        <v>1</v>
-      </c>
-      <c r="D111" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="112" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1438,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1446,15 +1460,15 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1462,15 +1476,15 @@
         <v>0</v>
       </c>
       <c r="D115" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C116" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D116" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="117" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1478,64 +1492,72 @@
         <v>30</v>
       </c>
       <c r="D117" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C118" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C118" s="3">
-        <v>0</v>
-      </c>
-      <c r="D118" t="s">
+    <row r="119" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="3">
+        <v>0</v>
+      </c>
+      <c r="D119" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="119" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C119" t="s">
-        <v>2</v>
-      </c>
-      <c r="D119" t="s">
+    <row r="120" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D120" t="s">
-        <v>2</v>
-      </c>
-      <c r="E120" t="s">
+    <row r="121" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" t="s">
         <v>25</v>
       </c>
-      <c r="F120" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="D121" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E121" s="2" t="s">
+      <c r="F121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D122" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F121" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C122" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
+      <c r="F122" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C123" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix after event. add noise timing etc.
</commit_message>
<xml_diff>
--- a/BlockPattern.xlsx
+++ b/BlockPattern.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1120" windowWidth="33940" windowHeight="22220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32640" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="81" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="63" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C63">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="D63" t="s">
         <v>18</v>

</xml_diff>